<commit_message>
changes to upload templates and gui, non public
</commit_message>
<xml_diff>
--- a/inst/shiny/uploadTemplates.xlsx
+++ b/inst/shiny/uploadTemplates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="5715" windowHeight="9525" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="5715" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="pcodeFile" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>USGS SID</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>analyzing entity code</t>
+  </si>
+  <si>
+    <t>qa code</t>
   </si>
 </sst>
 </file>
@@ -473,79 +476,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -658,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>